<commit_message>
Arquivos finais do trabalho
</commit_message>
<xml_diff>
--- a/Censo 2022 - Pirâmide etária - Rio de Janeiro (RJ).xlsx
+++ b/Censo 2022 - Pirâmide etária - Rio de Janeiro (RJ).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fidel\Dropbox\Pos_Insper_DataScience\MDCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984C4C05-1695-49EC-B634-587B81F6E2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76EB3CD-26DD-4667-AD5A-42319A9E8D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -512,15 +512,15 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B11" sqref="B11:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -560,7 +560,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -580,7 +580,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -600,7 +600,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -620,7 +620,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -640,7 +640,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -660,7 +660,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -680,7 +680,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -700,7 +700,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -720,7 +720,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -740,7 +740,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -760,7 +760,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -780,7 +780,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -800,7 +800,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -820,7 +820,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -840,7 +840,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -860,7 +860,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -880,7 +880,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -900,7 +900,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -920,7 +920,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -940,7 +940,7 @@
         <v>3304557</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -977,21 +977,21 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>SUM(B24:C24)</f>
-        <v>2765408</v>
+        <v>3553820</v>
       </c>
       <c r="B24">
-        <f>SUM(B13:B18)</f>
-        <v>1447380</v>
+        <f>SUM(B11:B18)</f>
+        <v>1880000</v>
       </c>
       <c r="C24">
-        <f>SUM(C13:C18)</f>
-        <v>1318028</v>
+        <f>SUM(C11:C18)</f>
+        <v>1673820</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f>A24/A23</f>
-        <v>0.44522761459377647</v>
+        <v>0.57216107037213126</v>
       </c>
       <c r="B25" t="s">
         <v>29</v>

</xml_diff>